<commit_message>
Done some analysis on most recurring words in Voynich across different clusters
</commit_message>
<xml_diff>
--- a/org.v4j/src/main/resources/Output/BlockWordEntropy.xlsx
+++ b/org.v4j/src/main/resources/Output/BlockWordEntropy.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="26">
   <si>
     <t>Cluster</t>
   </si>
@@ -93,6 +93,9 @@
   <si>
     <t>Bible_RND</t>
   </si>
+  <si>
+    <t>Completed.</t>
+  </si>
 </sst>
 </file>
 
@@ -152,13 +155,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -899,11 +899,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="175871488"/>
-        <c:axId val="175873024"/>
+        <c:axId val="145089664"/>
+        <c:axId val="145091200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="175871488"/>
+        <c:axId val="145089664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -912,7 +912,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="175873024"/>
+        <c:crossAx val="145091200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -920,7 +920,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="175873024"/>
+        <c:axId val="145091200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="13"/>
@@ -933,7 +933,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="175871488"/>
+        <c:crossAx val="145089664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1479,11 +1479,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="206403840"/>
-        <c:axId val="216201088"/>
+        <c:axId val="145351040"/>
+        <c:axId val="145352576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="206403840"/>
+        <c:axId val="145351040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1492,7 +1492,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="216201088"/>
+        <c:crossAx val="145352576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1500,7 +1500,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="216201088"/>
+        <c:axId val="145352576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
@@ -1513,7 +1513,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="206403840"/>
+        <c:crossAx val="145351040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1648,31 +1648,31 @@
                   <c:v>9.1580902947686003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.4297424807482</c:v>
+                  <c:v>12.436560200445999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.5932285287267</c:v>
+                  <c:v>12.5924059115725</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.5660540381704</c:v>
+                  <c:v>12.5643876960524</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.536247215689601</c:v>
+                  <c:v>12.534546067458599</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.506307581101201</c:v>
+                  <c:v>12.504570739324601</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12.4767462039393</c:v>
+                  <c:v>12.475480126596301</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12.446824840781201</c:v>
+                  <c:v>12.446566409065101</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12.4175888403814</c:v>
+                  <c:v>12.417852514886601</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12.388824538023201</c:v>
+                  <c:v>12.3885555039816</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1779,31 +1779,31 @@
                   <c:v>8.3831138877980607</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.332628719465101</c:v>
+                  <c:v>12.328979337635401</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.623512613562101</c:v>
+                  <c:v>12.623208637001399</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.5898851792894</c:v>
+                  <c:v>12.5908209309287</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.5521887595577</c:v>
+                  <c:v>12.553149275600401</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.515207030407099</c:v>
+                  <c:v>12.515453455389199</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12.4787696194761</c:v>
+                  <c:v>12.477758266443001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12.442425193330299</c:v>
+                  <c:v>12.4398308839811</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12.4059391933438</c:v>
+                  <c:v>12.4011461821541</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12.369324702408001</c:v>
+                  <c:v>12.362217815913301</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1841,7 +1841,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>8.8735133728721909</c:v>
+                  <c:v>8.8735133728721998</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>11.593725140943</c:v>
@@ -1907,13 +1907,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>8.8735133728721909</c:v>
+                  <c:v>8.8735133728721998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.0383634361059</c:v>
+                  <c:v>12.022942897264301</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.2809817472099</c:v>
+                  <c:v>12.279381106953799</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>12.2868465027355</c:v>
@@ -1974,28 +1974,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>8.1094259039789502</c:v>
+                  <c:v>7.9557104661710101</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.9395280636162</c:v>
+                  <c:v>10.872249220852799</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.714792075437799</c:v>
+                  <c:v>11.690350864914199</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.988287511958999</c:v>
+                  <c:v>11.9770729632263</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.098835107375599</c:v>
+                  <c:v>12.095310359482401</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.153769294288301</c:v>
+                  <c:v>12.151366891885999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12.186749446608999</c:v>
+                  <c:v>12.1851475243022</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12.207882406509899</c:v>
+                  <c:v>12.2074818457248</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>12.226166386511601</c:v>
@@ -2042,13 +2042,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>8.1094259039789502</c:v>
+                  <c:v>7.9557104661710101</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.939624670485401</c:v>
+                  <c:v>11.8918786744805</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.282333265317501</c:v>
+                  <c:v>12.2785807868257</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>12.2868465027355</c:v>
@@ -2086,11 +2086,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="43156992"/>
-        <c:axId val="43158528"/>
+        <c:axId val="145505664"/>
+        <c:axId val="145515648"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="43156992"/>
+        <c:axId val="145505664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2099,7 +2099,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43158528"/>
+        <c:crossAx val="145515648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2107,7 +2107,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="43158528"/>
+        <c:axId val="145515648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="13"/>
@@ -2120,7 +2120,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43156992"/>
+        <c:crossAx val="145505664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2262,31 +2262,31 @@
                   <c:v>9.0745342161384492</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.080803572365866</c:v>
+                  <c:v>12.08221475104815</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.170687141923251</c:v>
+                  <c:v>12.170521666611883</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.126183174577534</c:v>
+                  <c:v>12.125056282315349</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.080201311085084</c:v>
+                  <c:v>12.077750110637586</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.033764834316584</c:v>
+                  <c:v>12.030205484074633</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11.987418427796316</c:v>
+                  <c:v>11.982345348390368</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.940941240042617</c:v>
+                  <c:v>11.934425175148418</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11.894527756111799</c:v>
+                  <c:v>11.885803232839933</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11.848059358290802</c:v>
+                  <c:v>11.83688458221795</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2324,31 +2324,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>8.4607901783179553</c:v>
+                  <c:v>8.3375675939909382</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.267815430358</c:v>
+                  <c:v>11.219764822322174</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.885103853980899</c:v>
+                  <c:v>11.868741277008274</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.0851873394758</c:v>
+                  <c:v>12.077677176681226</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.1642026701247</c:v>
+                  <c:v>12.161539575601626</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.204657964382827</c:v>
+                  <c:v>12.203313882652525</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12.230137475865774</c:v>
+                  <c:v>12.229336514712376</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12.24597987533225</c:v>
+                  <c:v>12.245679454743424</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12.25722760292035</c:v>
+                  <c:v>12.257027282407526</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>12.265158591946724</c:v>
@@ -2390,16 +2390,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>8.4607901783179553</c:v>
+                  <c:v>8.3375675939909382</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.018842480958776</c:v>
+                  <c:v>11.973841479183877</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.28255786640775</c:v>
+                  <c:v>12.2797435075389</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.2868465027355</c:v>
+                  <c:v>12.28664638266345</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>12.2865577616086</c:v>
@@ -2434,11 +2434,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="42385792"/>
-        <c:axId val="42387328"/>
+        <c:axId val="145552512"/>
+        <c:axId val="145554048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="42385792"/>
+        <c:axId val="145552512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2447,7 +2447,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42387328"/>
+        <c:crossAx val="145554048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2455,7 +2455,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="42387328"/>
+        <c:axId val="145554048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="13"/>
@@ -2468,7 +2468,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42385792"/>
+        <c:crossAx val="145552512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2565,13 +2565,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>95249</xdr:colOff>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>47624</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>523874</xdr:colOff>
+      <xdr:colOff>523875</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>76199</xdr:rowOff>
     </xdr:to>
@@ -2600,15 +2600,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>66676</xdr:colOff>
+      <xdr:colOff>28575</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>28574</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3684,10 +3684,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A9" sqref="A9:XFD36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3739,31 +3739,31 @@
         <v>9.1580902947686003</v>
       </c>
       <c r="C2">
-        <v>12.4297424807482</v>
+        <v>12.436560200445999</v>
       </c>
       <c r="D2">
-        <v>12.5932285287267</v>
+        <v>12.5924059115725</v>
       </c>
       <c r="E2">
-        <v>12.5660540381704</v>
+        <v>12.5643876960524</v>
       </c>
       <c r="F2">
-        <v>12.536247215689601</v>
+        <v>12.534546067458599</v>
       </c>
       <c r="G2">
-        <v>12.506307581101201</v>
+        <v>12.504570739324601</v>
       </c>
       <c r="H2">
-        <v>12.4767462039393</v>
+        <v>12.475480126596301</v>
       </c>
       <c r="I2">
-        <v>12.446824840781201</v>
+        <v>12.446566409065101</v>
       </c>
       <c r="J2">
-        <v>12.4175888403814</v>
+        <v>12.417852514886601</v>
       </c>
       <c r="K2">
-        <v>12.388824538023201</v>
+        <v>12.3885555039816</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -3809,31 +3809,31 @@
         <v>8.3831138877980607</v>
       </c>
       <c r="C4">
-        <v>12.332628719465101</v>
+        <v>12.328979337635401</v>
       </c>
       <c r="D4">
-        <v>12.623512613562101</v>
+        <v>12.623208637001399</v>
       </c>
       <c r="E4">
-        <v>12.5898851792894</v>
+        <v>12.5908209309287</v>
       </c>
       <c r="F4">
-        <v>12.5521887595577</v>
+        <v>12.553149275600401</v>
       </c>
       <c r="G4">
-        <v>12.515207030407099</v>
+        <v>12.515453455389199</v>
       </c>
       <c r="H4">
-        <v>12.4787696194761</v>
+        <v>12.477758266443001</v>
       </c>
       <c r="I4">
-        <v>12.442425193330299</v>
+        <v>12.4398308839811</v>
       </c>
       <c r="J4">
-        <v>12.4059391933438</v>
+        <v>12.4011461821541</v>
       </c>
       <c r="K4">
-        <v>12.369324702408001</v>
+        <v>12.362217815913301</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -3841,7 +3841,7 @@
         <v>14</v>
       </c>
       <c r="B5">
-        <v>8.8735133728721909</v>
+        <v>8.8735133728721998</v>
       </c>
       <c r="C5">
         <v>11.593725140943</v>
@@ -3876,13 +3876,13 @@
         <v>18</v>
       </c>
       <c r="B6">
-        <v>8.8735133728721909</v>
+        <v>8.8735133728721998</v>
       </c>
       <c r="C6">
-        <v>12.0383634361059</v>
+        <v>12.022942897264301</v>
       </c>
       <c r="D6">
-        <v>12.2809817472099</v>
+        <v>12.279381106953799</v>
       </c>
       <c r="E6">
         <v>12.2868465027355</v>
@@ -3911,28 +3911,28 @@
         <v>16</v>
       </c>
       <c r="B7">
-        <v>8.1094259039789502</v>
+        <v>7.9557104661710101</v>
       </c>
       <c r="C7">
-        <v>10.9395280636162</v>
+        <v>10.872249220852799</v>
       </c>
       <c r="D7">
-        <v>11.714792075437799</v>
+        <v>11.690350864914199</v>
       </c>
       <c r="E7">
-        <v>11.988287511958999</v>
+        <v>11.9770729632263</v>
       </c>
       <c r="F7">
-        <v>12.098835107375599</v>
+        <v>12.095310359482401</v>
       </c>
       <c r="G7">
-        <v>12.153769294288301</v>
+        <v>12.151366891885999</v>
       </c>
       <c r="H7">
-        <v>12.186749446608999</v>
+        <v>12.1851475243022</v>
       </c>
       <c r="I7">
-        <v>12.207882406509899</v>
+        <v>12.2074818457248</v>
       </c>
       <c r="J7">
         <v>12.226166386511601</v>
@@ -3946,13 +3946,13 @@
         <v>20</v>
       </c>
       <c r="B8">
-        <v>8.1094259039789502</v>
+        <v>7.9557104661710101</v>
       </c>
       <c r="C8">
-        <v>11.939624670485401</v>
+        <v>11.8918786744805</v>
       </c>
       <c r="D8">
-        <v>12.282333265317501</v>
+        <v>12.2785807868257</v>
       </c>
       <c r="E8">
         <v>12.2868465027355</v>
@@ -3974,6 +3974,11 @@
       </c>
       <c r="K8">
         <v>12.2851131885001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -3987,7 +3992,7 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O2:P3"/>
+      <selection activeCell="A29" sqref="A29:K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3996,1023 +4001,1023 @@
     <col min="2" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B1">
         <v>9.1580902947686003</v>
       </c>
-      <c r="C1" s="2">
+      <c r="C1">
         <v>12.372907474091599</v>
       </c>
-      <c r="D1" s="2">
+      <c r="D1">
         <v>12.5935916154386</v>
       </c>
-      <c r="E1" s="2">
+      <c r="E1">
         <v>12.5708044377234</v>
       </c>
-      <c r="F1" s="2">
+      <c r="F1">
         <v>12.543998450133801</v>
       </c>
-      <c r="G1" s="2">
+      <c r="G1">
         <v>12.517915392917301</v>
       </c>
-      <c r="H1" s="2">
+      <c r="H1">
         <v>12.491602606696601</v>
       </c>
-      <c r="I1" s="2">
+      <c r="I1">
         <v>12.464800981655101</v>
       </c>
-      <c r="J1" s="2">
+      <c r="J1">
         <v>12.438012087652</v>
       </c>
-      <c r="K1" s="2">
+      <c r="K1">
         <v>12.4112461518398</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2">
         <v>9.1429813117594492</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <v>11.6428076513489</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2">
         <v>11.67914075447</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2">
         <v>11.6124077931392</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2">
         <v>11.5454471816777</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2">
         <v>11.4777582664434</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2">
         <v>11.411510988012401</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2">
         <v>11.348174867535199</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2">
         <v>11.2865577616084</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2">
         <v>11.2306209331296</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3">
         <v>9.0801121918337593</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3">
         <v>11.5660885140678</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3">
         <v>11.643057352048199</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3">
         <v>11.6105635039257</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3">
         <v>11.5783726913603</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3">
         <v>11.5464121951187</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3">
         <v>11.5156998382836</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3">
         <v>11.4853261892401</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3">
         <v>11.455840909126101</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3">
         <v>11.426264754702</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
         <v>8.3831138877980607</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>12.173838453572801</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4">
         <v>12.6083321454746</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4">
         <v>12.5936777733962</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4">
         <v>12.5586598670246</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4">
         <v>12.5230718269421</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4">
         <v>12.4875888463843</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4">
         <v>12.451983777229</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4">
         <v>12.416005780558701</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4">
         <v>12.3799198176477</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5">
         <v>9.0225654358041893</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5">
         <v>12.1314807164122</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5">
         <v>12.3098321268735</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5">
         <v>12.279900715803301</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5">
         <v>12.2458497710239</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5">
         <v>12.211888294545799</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5">
         <v>12.178042328864199</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5">
         <v>12.1446582428323</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5">
         <v>12.1127652818843</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5">
         <v>12.0808175276092</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6">
         <v>9.6603421748666296</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6">
         <v>12.1532137652624</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6">
         <v>12.204523139319599</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6">
         <v>12.1579784499444</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6">
         <v>12.110157018954499</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6">
         <v>12.063395081289</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6">
         <v>12.0178523319049</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6">
         <v>11.973338620801099</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6">
         <v>11.9288884393982</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6">
         <v>11.884552133988</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="1">
         <f>AVERAGE(B1:B6)</f>
         <v>9.0745342161384475</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="1">
         <f t="shared" ref="C7:K7" si="0">AVERAGE(C1:C6)</f>
         <v>12.006722762459283</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="1">
         <f t="shared" si="0"/>
         <v>12.173079522270749</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="1">
         <f t="shared" si="0"/>
         <v>12.137555445655366</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="1">
         <f t="shared" si="0"/>
         <v>12.097080830029133</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="1">
         <f t="shared" si="0"/>
         <v>12.056740176209383</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="1">
         <f t="shared" si="0"/>
         <v>12.017049490024334</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="1">
         <f t="shared" si="0"/>
         <v>11.978047113215466</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="1">
         <f t="shared" si="0"/>
         <v>11.939678376704615</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7" s="1">
         <f t="shared" si="0"/>
         <v>11.902236886486049</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8">
         <v>9.1580902947686003</v>
       </c>
-      <c r="C8" s="1">
-        <v>12.4297424807482</v>
-      </c>
-      <c r="D8" s="1">
-        <v>12.5932285287267</v>
-      </c>
-      <c r="E8" s="1">
-        <v>12.5660540381704</v>
-      </c>
-      <c r="F8" s="1">
-        <v>12.536247215689601</v>
-      </c>
-      <c r="G8" s="1">
-        <v>12.506307581101201</v>
-      </c>
-      <c r="H8" s="1">
-        <v>12.4767462039393</v>
-      </c>
-      <c r="I8" s="1">
-        <v>12.446824840781201</v>
-      </c>
-      <c r="J8" s="1">
-        <v>12.4175888403814</v>
-      </c>
-      <c r="K8" s="1">
-        <v>12.388824538023201</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="C8">
+        <v>12.436560200445999</v>
+      </c>
+      <c r="D8">
+        <v>12.5924059115725</v>
+      </c>
+      <c r="E8">
+        <v>12.5643876960524</v>
+      </c>
+      <c r="F8">
+        <v>12.534546067458599</v>
+      </c>
+      <c r="G8">
+        <v>12.504570739324601</v>
+      </c>
+      <c r="H8">
+        <v>12.475480126596301</v>
+      </c>
+      <c r="I8">
+        <v>12.446566409065101</v>
+      </c>
+      <c r="J8">
+        <v>12.417852514886601</v>
+      </c>
+      <c r="K8">
+        <v>12.3885555039816</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9">
         <v>9.1429813117594492</v>
       </c>
-      <c r="C9" s="1">
-        <v>11.672272686249499</v>
-      </c>
-      <c r="D9" s="1">
-        <v>11.662496595535099</v>
-      </c>
-      <c r="E9" s="1">
-        <v>11.5854320515938</v>
-      </c>
-      <c r="F9" s="1">
-        <v>11.5053153561361</v>
-      </c>
-      <c r="G9" s="1">
-        <v>11.423641195075801</v>
-      </c>
-      <c r="H9" s="1">
-        <v>11.3431857154475</v>
-      </c>
-      <c r="I9" s="1">
-        <v>11.263269200373101</v>
-      </c>
-      <c r="J9" s="1">
-        <v>11.184255495405001</v>
-      </c>
-      <c r="K9" s="1">
-        <v>11.1045987535647</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="C9">
+        <v>11.6830960325077</v>
+      </c>
+      <c r="D9">
+        <v>11.661778097772601</v>
+      </c>
+      <c r="E9">
+        <v>11.577900836886499</v>
+      </c>
+      <c r="F9">
+        <v>11.493855449241</v>
+      </c>
+      <c r="G9">
+        <v>11.4099212412504</v>
+      </c>
+      <c r="H9">
+        <v>11.3236177632911</v>
+      </c>
+      <c r="I9">
+        <v>11.236014191900299</v>
+      </c>
+      <c r="J9">
+        <v>11.145295334934</v>
+      </c>
+      <c r="K9">
+        <v>11.0532471259122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10">
         <v>9.0801121918337699</v>
       </c>
-      <c r="C10" s="1">
-        <v>11.614739501608099</v>
-      </c>
-      <c r="D10" s="1">
-        <v>11.6375305515254</v>
-      </c>
-      <c r="E10" s="1">
-        <v>11.599447981528201</v>
-      </c>
-      <c r="F10" s="1">
-        <v>11.5612879451641</v>
-      </c>
-      <c r="G10" s="1">
-        <v>11.5230718269404</v>
-      </c>
-      <c r="H10" s="1">
-        <v>11.484319423644299</v>
-      </c>
-      <c r="I10" s="1">
-        <v>11.445532219028401</v>
-      </c>
-      <c r="J10" s="1">
-        <v>11.406736482691599</v>
-      </c>
-      <c r="K10" s="1">
-        <v>11.368506461507399</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="C10">
+        <v>11.6074938102125</v>
+      </c>
+      <c r="D10">
+        <v>11.638888382252199</v>
+      </c>
+      <c r="E10">
+        <v>11.600842114388</v>
+      </c>
+      <c r="F10">
+        <v>11.5622424242208</v>
+      </c>
+      <c r="G10">
+        <v>11.523561956057801</v>
+      </c>
+      <c r="H10">
+        <v>11.4848228942619</v>
+      </c>
+      <c r="I10">
+        <v>11.447599858280601</v>
+      </c>
+      <c r="J10">
+        <v>11.4104513515042</v>
+      </c>
+      <c r="K10">
+        <v>11.3728650601127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11">
         <v>8.3831138877980607</v>
       </c>
-      <c r="C11" s="1">
-        <v>12.332628719465101</v>
-      </c>
-      <c r="D11" s="1">
-        <v>12.623512613562101</v>
-      </c>
-      <c r="E11" s="1">
-        <v>12.5898851792894</v>
-      </c>
-      <c r="F11" s="1">
-        <v>12.5521887595577</v>
-      </c>
-      <c r="G11" s="1">
-        <v>12.515207030407099</v>
-      </c>
-      <c r="H11" s="1">
-        <v>12.4787696194761</v>
-      </c>
-      <c r="I11" s="1">
-        <v>12.442425193330299</v>
-      </c>
-      <c r="J11" s="1">
-        <v>12.4059391933438</v>
-      </c>
-      <c r="K11" s="1">
-        <v>12.369324702408001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="C11">
+        <v>12.328979337635401</v>
+      </c>
+      <c r="D11">
+        <v>12.623208637001399</v>
+      </c>
+      <c r="E11">
+        <v>12.5908209309287</v>
+      </c>
+      <c r="F11">
+        <v>12.553149275600401</v>
+      </c>
+      <c r="G11">
+        <v>12.515453455389199</v>
+      </c>
+      <c r="H11">
+        <v>12.477758266443001</v>
+      </c>
+      <c r="I11">
+        <v>12.4398308839811</v>
+      </c>
+      <c r="J11">
+        <v>12.4011461821541</v>
+      </c>
+      <c r="K11">
+        <v>12.362217815913301</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
         <v>9.0225654358041893</v>
       </c>
-      <c r="C12" s="1">
-        <v>12.2325287612039</v>
-      </c>
-      <c r="D12" s="1">
-        <v>12.307375554574</v>
-      </c>
-      <c r="E12" s="1">
-        <v>12.269711121143301</v>
-      </c>
-      <c r="F12" s="1">
-        <v>12.2324209271763</v>
-      </c>
-      <c r="G12" s="1">
-        <v>12.1947568544217</v>
-      </c>
-      <c r="H12" s="1">
-        <v>12.1567151442244</v>
-      </c>
-      <c r="I12" s="1">
-        <v>12.117967703718399</v>
-      </c>
-      <c r="J12" s="1">
-        <v>12.078817949962399</v>
-      </c>
-      <c r="K12" s="1">
-        <v>12.038918989293499</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="C12">
+        <v>12.2267125222223</v>
+      </c>
+      <c r="D12">
+        <v>12.3084039296191</v>
+      </c>
+      <c r="E12">
+        <v>12.272046524388999</v>
+      </c>
+      <c r="F12">
+        <v>12.233919208588301</v>
+      </c>
+      <c r="G12">
+        <v>12.195679785495299</v>
+      </c>
+      <c r="H12">
+        <v>12.1579784499444</v>
+      </c>
+      <c r="I12">
+        <v>12.1199137854518</v>
+      </c>
+      <c r="J12">
+        <v>12.082481727863099</v>
+      </c>
+      <c r="K12">
+        <v>12.044735626056299</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13">
         <v>9.6603421748666296</v>
       </c>
-      <c r="C13" s="1">
-        <v>12.2029092849204</v>
-      </c>
-      <c r="D13" s="1">
-        <v>12.1999790076162</v>
-      </c>
-      <c r="E13" s="1">
-        <v>12.146568675740101</v>
-      </c>
-      <c r="F13" s="1">
-        <v>12.093747662786701</v>
-      </c>
-      <c r="G13" s="1">
-        <v>12.0396045179533</v>
-      </c>
-      <c r="H13" s="1">
-        <v>11.9847744600463</v>
-      </c>
-      <c r="I13" s="1">
-        <v>11.9296282830243</v>
-      </c>
-      <c r="J13" s="1">
-        <v>11.8738285748866</v>
-      </c>
-      <c r="K13" s="1">
-        <v>11.818182704948001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="C13">
+        <v>12.210446603265</v>
+      </c>
+      <c r="D13">
+        <v>12.1984450414535</v>
+      </c>
+      <c r="E13">
+        <v>12.144339591247499</v>
+      </c>
+      <c r="F13">
+        <v>12.088788238716401</v>
+      </c>
+      <c r="G13">
+        <v>12.0320457269305</v>
+      </c>
+      <c r="H13">
+        <v>11.9744145898055</v>
+      </c>
+      <c r="I13">
+        <v>11.916625922211599</v>
+      </c>
+      <c r="J13">
+        <v>11.857592285697599</v>
+      </c>
+      <c r="K13">
+        <v>11.799686361331601</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="1">
         <f>AVERAGE(B8:B13)</f>
         <v>9.0745342161384492</v>
       </c>
-      <c r="C14" s="4">
-        <f t="shared" ref="C14" si="1">AVERAGE(C8:C13)</f>
-        <v>12.080803572365866</v>
-      </c>
-      <c r="D14" s="4">
-        <f t="shared" ref="D14" si="2">AVERAGE(D8:D13)</f>
-        <v>12.170687141923251</v>
-      </c>
-      <c r="E14" s="4">
-        <f t="shared" ref="E14" si="3">AVERAGE(E8:E13)</f>
-        <v>12.126183174577534</v>
-      </c>
-      <c r="F14" s="4">
-        <f t="shared" ref="F14" si="4">AVERAGE(F8:F13)</f>
-        <v>12.080201311085084</v>
-      </c>
-      <c r="G14" s="4">
-        <f t="shared" ref="G14" si="5">AVERAGE(G8:G13)</f>
-        <v>12.033764834316584</v>
-      </c>
-      <c r="H14" s="4">
-        <f t="shared" ref="H14" si="6">AVERAGE(H8:H13)</f>
-        <v>11.987418427796316</v>
-      </c>
-      <c r="I14" s="4">
-        <f t="shared" ref="I14" si="7">AVERAGE(I8:I13)</f>
-        <v>11.940941240042617</v>
-      </c>
-      <c r="J14" s="4">
-        <f t="shared" ref="J14" si="8">AVERAGE(J8:J13)</f>
-        <v>11.894527756111799</v>
-      </c>
-      <c r="K14" s="4">
-        <f t="shared" ref="K14" si="9">AVERAGE(K8:K13)</f>
-        <v>11.848059358290802</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="C14" s="1">
+        <f>AVERAGE(C8:C13)</f>
+        <v>12.08221475104815</v>
+      </c>
+      <c r="D14" s="1">
+        <f>AVERAGE(D8:D13)</f>
+        <v>12.170521666611883</v>
+      </c>
+      <c r="E14" s="1">
+        <f>AVERAGE(E8:E13)</f>
+        <v>12.125056282315349</v>
+      </c>
+      <c r="F14" s="1">
+        <f>AVERAGE(F8:F13)</f>
+        <v>12.077750110637586</v>
+      </c>
+      <c r="G14" s="1">
+        <f>AVERAGE(G8:G13)</f>
+        <v>12.030205484074633</v>
+      </c>
+      <c r="H14" s="1">
+        <f>AVERAGE(H8:H13)</f>
+        <v>11.982345348390368</v>
+      </c>
+      <c r="I14" s="1">
+        <f>AVERAGE(I8:I13)</f>
+        <v>11.934425175148418</v>
+      </c>
+      <c r="J14" s="1">
+        <f>AVERAGE(J8:J13)</f>
+        <v>11.885803232839933</v>
+      </c>
+      <c r="K14" s="1">
+        <f>AVERAGE(K8:K13)</f>
+        <v>11.83688458221795</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="2">
-        <v>8.5417649176750707</v>
-      </c>
-      <c r="C15" s="2">
-        <v>11.266373778533101</v>
-      </c>
-      <c r="D15" s="2">
-        <v>11.901377272424799</v>
-      </c>
-      <c r="E15" s="2">
-        <v>12.1069456899589</v>
-      </c>
-      <c r="F15" s="2">
-        <v>12.1801289098153</v>
-      </c>
-      <c r="G15" s="2">
-        <v>12.2168424180238</v>
-      </c>
-      <c r="H15" s="2">
-        <v>12.2403999947828</v>
-      </c>
-      <c r="I15" s="2">
+      <c r="B15">
+        <v>8.3767549134133805</v>
+      </c>
+      <c r="C15">
+        <v>11.207857445315501</v>
+      </c>
+      <c r="D15">
+        <v>11.8792498034778</v>
+      </c>
+      <c r="E15">
+        <v>12.096617564989099</v>
+      </c>
+      <c r="F15">
+        <v>12.1759746088741</v>
+      </c>
+      <c r="G15">
+        <v>12.216041617223</v>
+      </c>
+      <c r="H15">
+        <v>12.239999514206101</v>
+      </c>
+      <c r="I15">
         <v>12.256230396208901</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15">
         <v>12.2671613033916</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K15">
         <v>12.2745883788401</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="2">
-        <v>8.8735133728721909</v>
-      </c>
-      <c r="C16" s="2">
+      <c r="B16">
+        <v>8.8735133728721998</v>
+      </c>
+      <c r="C16">
         <v>11.593725140943</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16">
         <v>12.035289964404599</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16">
         <v>12.1628844968296</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16">
         <v>12.216975759779301</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16">
         <v>12.244945125788099</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16">
         <v>12.2637961026506</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16">
         <v>12.2737493421608</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J16">
         <v>12.2785964960147</v>
       </c>
-      <c r="K16" s="2">
+      <c r="K16">
         <v>12.281433659753</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="2">
-        <v>8.3184565187456094</v>
-      </c>
-      <c r="C17" s="2">
-        <v>11.271634738339699</v>
-      </c>
-      <c r="D17" s="2">
-        <v>11.888956103656399</v>
-      </c>
-      <c r="E17" s="2">
-        <v>12.0826316591557</v>
-      </c>
-      <c r="F17" s="2">
-        <v>12.1608709035286</v>
-      </c>
-      <c r="G17" s="2">
-        <v>12.2030750194311</v>
-      </c>
-      <c r="H17" s="2">
-        <v>12.2296043594207</v>
-      </c>
-      <c r="I17" s="2">
-        <v>12.2460573564494</v>
-      </c>
-      <c r="J17" s="2">
-        <v>12.2569862257635</v>
-      </c>
-      <c r="K17" s="2">
+      <c r="B17">
+        <v>8.1442916235071596</v>
+      </c>
+      <c r="C17">
+        <v>11.205227482177399</v>
+      </c>
+      <c r="D17">
+        <v>11.8700744752365</v>
+      </c>
+      <c r="E17">
+        <v>12.0741336816799</v>
+      </c>
+      <c r="F17">
+        <v>12.157897574270701</v>
+      </c>
+      <c r="G17">
+        <v>12.200901895713001</v>
+      </c>
+      <c r="H17">
+        <v>12.2284029176906</v>
+      </c>
+      <c r="I17">
+        <v>12.2452562348792</v>
+      </c>
+      <c r="J17">
+        <v>12.256184943712199</v>
+      </c>
+      <c r="K17">
         <v>12.265515204623499</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="2">
-        <v>8.1094259039789502</v>
-      </c>
-      <c r="C18" s="2">
-        <v>10.9395280636162</v>
-      </c>
-      <c r="D18" s="2">
-        <v>11.714792075437799</v>
-      </c>
-      <c r="E18" s="2">
-        <v>11.988287511958999</v>
-      </c>
-      <c r="F18" s="2">
-        <v>12.098835107375599</v>
-      </c>
-      <c r="G18" s="2">
-        <v>12.153769294288301</v>
-      </c>
-      <c r="H18" s="2">
-        <v>12.186749446608999</v>
-      </c>
-      <c r="I18" s="2">
-        <v>12.207882406509899</v>
-      </c>
-      <c r="J18" s="2">
+      <c r="B18">
+        <v>7.9557104661710101</v>
+      </c>
+      <c r="C18">
+        <v>10.872249220852799</v>
+      </c>
+      <c r="D18">
+        <v>11.690350864914199</v>
+      </c>
+      <c r="E18">
+        <v>11.9770729632263</v>
+      </c>
+      <c r="F18">
+        <v>12.095310359482401</v>
+      </c>
+      <c r="G18">
+        <v>12.151366891885999</v>
+      </c>
+      <c r="H18">
+        <v>12.1851475243022</v>
+      </c>
+      <c r="I18">
+        <v>12.2074818457248</v>
+      </c>
+      <c r="J18">
         <v>12.226166386511601</v>
       </c>
-      <c r="K18" s="2">
+      <c r="K18">
         <v>12.2390971245703</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="1">
         <f>AVERAGE(B15:B18)</f>
-        <v>8.4607901783179553</v>
-      </c>
-      <c r="C19" s="3">
-        <f t="shared" ref="C19:K19" si="10">AVERAGE(C15:C18)</f>
-        <v>11.267815430358</v>
-      </c>
-      <c r="D19" s="3">
-        <f t="shared" si="10"/>
-        <v>11.885103853980899</v>
-      </c>
-      <c r="E19" s="3">
-        <f t="shared" si="10"/>
-        <v>12.0851873394758</v>
-      </c>
-      <c r="F19" s="3">
-        <f t="shared" si="10"/>
-        <v>12.1642026701247</v>
-      </c>
-      <c r="G19" s="3">
-        <f t="shared" si="10"/>
-        <v>12.204657964382827</v>
-      </c>
-      <c r="H19" s="3">
-        <f t="shared" si="10"/>
-        <v>12.230137475865774</v>
-      </c>
-      <c r="I19" s="3">
-        <f t="shared" si="10"/>
-        <v>12.24597987533225</v>
-      </c>
-      <c r="J19" s="3">
-        <f t="shared" si="10"/>
-        <v>12.25722760292035</v>
-      </c>
-      <c r="K19" s="3">
-        <f t="shared" si="10"/>
+        <v>8.3375675939909382</v>
+      </c>
+      <c r="C19" s="1">
+        <f>AVERAGE(C15:C18)</f>
+        <v>11.219764822322174</v>
+      </c>
+      <c r="D19" s="1">
+        <f>AVERAGE(D15:D18)</f>
+        <v>11.868741277008274</v>
+      </c>
+      <c r="E19" s="1">
+        <f>AVERAGE(E15:E18)</f>
+        <v>12.077677176681226</v>
+      </c>
+      <c r="F19" s="1">
+        <f>AVERAGE(F15:F18)</f>
+        <v>12.161539575601626</v>
+      </c>
+      <c r="G19" s="1">
+        <f>AVERAGE(G15:G18)</f>
+        <v>12.203313882652525</v>
+      </c>
+      <c r="H19" s="1">
+        <f>AVERAGE(H15:H18)</f>
+        <v>12.229336514712376</v>
+      </c>
+      <c r="I19" s="1">
+        <f>AVERAGE(I15:I18)</f>
+        <v>12.245679454743424</v>
+      </c>
+      <c r="J19" s="1">
+        <f>AVERAGE(J15:J18)</f>
+        <v>12.257027282407526</v>
+      </c>
+      <c r="K19" s="1">
+        <f>AVERAGE(K15:K18)</f>
         <v>12.265158591946724</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>8.3767549134133805</v>
+      </c>
+      <c r="C20">
+        <v>12.0325885328725</v>
+      </c>
+      <c r="D20">
+        <v>12.2815329451895</v>
+      </c>
+      <c r="E20">
+        <v>12.286446262591401</v>
+      </c>
+      <c r="F20">
+        <v>12.2865577616086</v>
+      </c>
+      <c r="G20">
+        <v>12.2862689626789</v>
+      </c>
+      <c r="H20">
+        <v>12.285980105927401</v>
+      </c>
+      <c r="I20">
+        <v>12.285691191330701</v>
+      </c>
+      <c r="J20">
+        <v>12.285402218861501</v>
+      </c>
+      <c r="K20">
+        <v>12.2851131885001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="1">
-        <v>8.8735133728721909</v>
-      </c>
-      <c r="C20" s="1">
-        <v>12.0383634361059</v>
-      </c>
-      <c r="D20" s="1">
-        <v>12.2809817472099</v>
-      </c>
-      <c r="E20" s="1">
+      <c r="B21">
+        <v>8.8735133728721998</v>
+      </c>
+      <c r="C21">
+        <v>12.022942897264301</v>
+      </c>
+      <c r="D21">
+        <v>12.279381106953799</v>
+      </c>
+      <c r="E21">
         <v>12.2868465027355</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F21">
         <v>12.2865577616086</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G21">
         <v>12.2862689626789</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H21">
         <v>12.285980105927401</v>
       </c>
-      <c r="I20" s="1">
+      <c r="I21">
         <v>12.285691191330701</v>
       </c>
-      <c r="J20" s="1">
+      <c r="J21">
         <v>12.285402218861501</v>
       </c>
-      <c r="K20" s="1">
+      <c r="K21">
         <v>12.2851131885001</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="1">
-        <v>8.5417649176750707</v>
-      </c>
-      <c r="C21" s="1">
-        <v>12.0801491482031</v>
-      </c>
-      <c r="D21" s="1">
-        <v>12.2855345458297</v>
-      </c>
-      <c r="E21" s="1">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>8.1442916235071596</v>
+      </c>
+      <c r="C22">
+        <v>11.947955812118201</v>
+      </c>
+      <c r="D22">
+        <v>12.279479191186599</v>
+      </c>
+      <c r="E22">
+        <v>12.286446262591401</v>
+      </c>
+      <c r="F22">
+        <v>12.2865577616086</v>
+      </c>
+      <c r="G22">
+        <v>12.2862689626789</v>
+      </c>
+      <c r="H22">
+        <v>12.285980105927401</v>
+      </c>
+      <c r="I22">
+        <v>12.285691191330701</v>
+      </c>
+      <c r="J22">
+        <v>12.285402218861501</v>
+      </c>
+      <c r="K22">
+        <v>12.2851131885001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23">
+        <v>7.9557104661710101</v>
+      </c>
+      <c r="C23">
+        <v>11.8918786744805</v>
+      </c>
+      <c r="D23">
+        <v>12.2785807868257</v>
+      </c>
+      <c r="E23">
         <v>12.2868465027355</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F23">
         <v>12.2865577616086</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G23">
         <v>12.2862689626789</v>
       </c>
-      <c r="H21" s="1">
+      <c r="H23">
         <v>12.285980105927401</v>
       </c>
-      <c r="I21" s="1">
+      <c r="I23">
         <v>12.285691191330701</v>
       </c>
-      <c r="J21" s="1">
+      <c r="J23">
         <v>12.285402218861501</v>
       </c>
-      <c r="K21" s="1">
+      <c r="K23">
         <v>12.2851131885001</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="1">
-        <v>8.3184565187456094</v>
-      </c>
-      <c r="C22" s="1">
-        <v>12.0172326690407</v>
-      </c>
-      <c r="D22" s="1">
-        <v>12.2813819072739</v>
-      </c>
-      <c r="E22" s="1">
-        <v>12.2868465027355</v>
-      </c>
-      <c r="F22" s="1">
+    <row r="24" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="1">
+        <f>AVERAGE(B20:B23)</f>
+        <v>8.3375675939909382</v>
+      </c>
+      <c r="C24" s="1">
+        <f t="shared" ref="C24" si="1">AVERAGE(C20:C23)</f>
+        <v>11.973841479183877</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" ref="D24" si="2">AVERAGE(D20:D23)</f>
+        <v>12.2797435075389</v>
+      </c>
+      <c r="E24" s="1">
+        <f t="shared" ref="E24" si="3">AVERAGE(E20:E23)</f>
+        <v>12.28664638266345</v>
+      </c>
+      <c r="F24" s="1">
+        <f t="shared" ref="F24" si="4">AVERAGE(F20:F23)</f>
         <v>12.2865577616086</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G24" s="1">
+        <f t="shared" ref="G24" si="5">AVERAGE(G20:G23)</f>
         <v>12.2862689626789</v>
       </c>
-      <c r="H22" s="1">
+      <c r="H24" s="1">
+        <f t="shared" ref="H24" si="6">AVERAGE(H20:H23)</f>
         <v>12.285980105927401</v>
       </c>
-      <c r="I22" s="1">
+      <c r="I24" s="1">
+        <f t="shared" ref="I24" si="7">AVERAGE(I20:I23)</f>
         <v>12.285691191330701</v>
       </c>
-      <c r="J22" s="1">
+      <c r="J24" s="1">
+        <f t="shared" ref="J24" si="8">AVERAGE(J20:J23)</f>
         <v>12.285402218861501</v>
       </c>
-      <c r="K22" s="1">
+      <c r="K24" s="1">
+        <f t="shared" ref="K24" si="9">AVERAGE(K20:K23)</f>
         <v>12.2851131885001</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="1">
-        <v>8.1094259039789502</v>
-      </c>
-      <c r="C23" s="1">
-        <v>11.939624670485401</v>
-      </c>
-      <c r="D23" s="1">
-        <v>12.282333265317501</v>
-      </c>
-      <c r="E23" s="1">
-        <v>12.2868465027355</v>
-      </c>
-      <c r="F23" s="1">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="2">
+        <v>9.0745342161384475</v>
+      </c>
+      <c r="C26" s="2">
+        <v>12.006722762459283</v>
+      </c>
+      <c r="D26" s="2">
+        <v>12.173079522270749</v>
+      </c>
+      <c r="E26" s="2">
+        <v>12.137555445655366</v>
+      </c>
+      <c r="F26" s="2">
+        <v>12.097080830029133</v>
+      </c>
+      <c r="G26" s="2">
+        <v>12.056740176209383</v>
+      </c>
+      <c r="H26" s="2">
+        <v>12.017049490024334</v>
+      </c>
+      <c r="I26" s="2">
+        <v>11.978047113215466</v>
+      </c>
+      <c r="J26" s="2">
+        <v>11.939678376704615</v>
+      </c>
+      <c r="K26" s="2">
+        <v>11.902236886486049</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="2">
+        <v>9.0745342161384492</v>
+      </c>
+      <c r="C27" s="2">
+        <v>12.08221475104815</v>
+      </c>
+      <c r="D27" s="2">
+        <v>12.170521666611883</v>
+      </c>
+      <c r="E27" s="2">
+        <v>12.125056282315349</v>
+      </c>
+      <c r="F27" s="2">
+        <v>12.077750110637586</v>
+      </c>
+      <c r="G27" s="2">
+        <v>12.030205484074633</v>
+      </c>
+      <c r="H27" s="2">
+        <v>11.982345348390368</v>
+      </c>
+      <c r="I27" s="2">
+        <v>11.934425175148418</v>
+      </c>
+      <c r="J27" s="2">
+        <v>11.885803232839933</v>
+      </c>
+      <c r="K27" s="2">
+        <v>11.83688458221795</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="2">
+        <v>8.3375675939909382</v>
+      </c>
+      <c r="C28" s="2">
+        <v>11.219764822322174</v>
+      </c>
+      <c r="D28" s="2">
+        <v>11.868741277008274</v>
+      </c>
+      <c r="E28" s="2">
+        <v>12.077677176681226</v>
+      </c>
+      <c r="F28" s="2">
+        <v>12.161539575601626</v>
+      </c>
+      <c r="G28" s="2">
+        <v>12.203313882652525</v>
+      </c>
+      <c r="H28" s="2">
+        <v>12.229336514712376</v>
+      </c>
+      <c r="I28" s="2">
+        <v>12.245679454743424</v>
+      </c>
+      <c r="J28" s="2">
+        <v>12.257027282407526</v>
+      </c>
+      <c r="K28" s="2">
+        <v>12.265158591946724</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="2">
+        <v>8.3375675939909382</v>
+      </c>
+      <c r="C29" s="2">
+        <v>11.973841479183877</v>
+      </c>
+      <c r="D29" s="2">
+        <v>12.2797435075389</v>
+      </c>
+      <c r="E29" s="2">
+        <v>12.28664638266345</v>
+      </c>
+      <c r="F29" s="2">
         <v>12.2865577616086</v>
       </c>
-      <c r="G23" s="1">
+      <c r="G29" s="2">
         <v>12.2862689626789</v>
       </c>
-      <c r="H23" s="1">
+      <c r="H29" s="2">
         <v>12.285980105927401</v>
       </c>
-      <c r="I23" s="1">
+      <c r="I29" s="2">
         <v>12.285691191330701</v>
       </c>
-      <c r="J23" s="1">
+      <c r="J29" s="2">
         <v>12.285402218861501</v>
       </c>
-      <c r="K23" s="1">
-        <v>12.2851131885001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="5">
-        <f>AVERAGE(B20:B23)</f>
-        <v>8.4607901783179553</v>
-      </c>
-      <c r="C24" s="5">
-        <f t="shared" ref="C24" si="11">AVERAGE(C20:C23)</f>
-        <v>12.018842480958776</v>
-      </c>
-      <c r="D24" s="5">
-        <f t="shared" ref="D24" si="12">AVERAGE(D20:D23)</f>
-        <v>12.28255786640775</v>
-      </c>
-      <c r="E24" s="5">
-        <f t="shared" ref="E24" si="13">AVERAGE(E20:E23)</f>
-        <v>12.2868465027355</v>
-      </c>
-      <c r="F24" s="5">
-        <f t="shared" ref="F24" si="14">AVERAGE(F20:F23)</f>
-        <v>12.2865577616086</v>
-      </c>
-      <c r="G24" s="5">
-        <f t="shared" ref="G24" si="15">AVERAGE(G20:G23)</f>
-        <v>12.2862689626789</v>
-      </c>
-      <c r="H24" s="5">
-        <f t="shared" ref="H24" si="16">AVERAGE(H20:H23)</f>
-        <v>12.285980105927401</v>
-      </c>
-      <c r="I24" s="5">
-        <f t="shared" ref="I24" si="17">AVERAGE(I20:I23)</f>
-        <v>12.285691191330701</v>
-      </c>
-      <c r="J24" s="5">
-        <f t="shared" ref="J24" si="18">AVERAGE(J20:J23)</f>
-        <v>12.285402218861501</v>
-      </c>
-      <c r="K24" s="5">
-        <f t="shared" ref="K24" si="19">AVERAGE(K20:K23)</f>
-        <v>12.2851131885001</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26">
-        <v>9.0745342161384475</v>
-      </c>
-      <c r="C26">
-        <v>12.006722762459283</v>
-      </c>
-      <c r="D26">
-        <v>12.173079522270749</v>
-      </c>
-      <c r="E26">
-        <v>12.137555445655366</v>
-      </c>
-      <c r="F26">
-        <v>12.097080830029133</v>
-      </c>
-      <c r="G26">
-        <v>12.056740176209383</v>
-      </c>
-      <c r="H26">
-        <v>12.017049490024334</v>
-      </c>
-      <c r="I26">
-        <v>11.978047113215466</v>
-      </c>
-      <c r="J26">
-        <v>11.939678376704615</v>
-      </c>
-      <c r="K26">
-        <v>11.902236886486049</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27">
-        <v>9.0745342161384492</v>
-      </c>
-      <c r="C27">
-        <v>12.080803572365866</v>
-      </c>
-      <c r="D27">
-        <v>12.170687141923251</v>
-      </c>
-      <c r="E27">
-        <v>12.126183174577534</v>
-      </c>
-      <c r="F27">
-        <v>12.080201311085084</v>
-      </c>
-      <c r="G27">
-        <v>12.033764834316584</v>
-      </c>
-      <c r="H27">
-        <v>11.987418427796316</v>
-      </c>
-      <c r="I27">
-        <v>11.940941240042617</v>
-      </c>
-      <c r="J27">
-        <v>11.894527756111799</v>
-      </c>
-      <c r="K27">
-        <v>11.848059358290802</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>23</v>
-      </c>
-      <c r="B28">
-        <v>8.4607901783179553</v>
-      </c>
-      <c r="C28">
-        <v>11.267815430358</v>
-      </c>
-      <c r="D28">
-        <v>11.885103853980899</v>
-      </c>
-      <c r="E28">
-        <v>12.0851873394758</v>
-      </c>
-      <c r="F28">
-        <v>12.1642026701247</v>
-      </c>
-      <c r="G28">
-        <v>12.204657964382827</v>
-      </c>
-      <c r="H28">
-        <v>12.230137475865774</v>
-      </c>
-      <c r="I28">
-        <v>12.24597987533225</v>
-      </c>
-      <c r="J28">
-        <v>12.25722760292035</v>
-      </c>
-      <c r="K28">
-        <v>12.265158591946724</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29">
-        <v>8.4607901783179553</v>
-      </c>
-      <c r="C29">
-        <v>12.018842480958776</v>
-      </c>
-      <c r="D29">
-        <v>12.28255786640775</v>
-      </c>
-      <c r="E29">
-        <v>12.2868465027355</v>
-      </c>
-      <c r="F29">
-        <v>12.2865577616086</v>
-      </c>
-      <c r="G29">
-        <v>12.2862689626789</v>
-      </c>
-      <c r="H29">
-        <v>12.285980105927401</v>
-      </c>
-      <c r="I29">
-        <v>12.285691191330701</v>
-      </c>
-      <c r="J29">
-        <v>12.285402218861501</v>
-      </c>
-      <c r="K29">
+      <c r="K29" s="2">
         <v>12.2851131885001</v>
       </c>
     </row>

</xml_diff>